<commit_message>
Creating Supplemental Materials for OSF
</commit_message>
<xml_diff>
--- a/Manuscript Analysis/Shared Data/Speaker Baselines.xlsx
+++ b/Manuscript Analysis/Shared Data/Speaker Baselines.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meganhirsch/Dropbox (Micah Hirsch FSU)/Spring 2021 DIS Hirsch and Thompson/DIS_Project/Data/Shared Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meh17e/Documents/GitHub Repositories/SLP-Intelligibility-of-Dysarthric-Speech/Manuscript Analysis/Shared Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04285EEF-33D4-0D4D-9AE3-DBC8F901E405}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{507F2E26-7C25-194E-8B42-1DA3FA22A414}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7280" yWindow="860" windowWidth="21320" windowHeight="16860" xr2:uid="{CFB46327-7120-EF4D-A752-995E394E2DEB}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Speaker</t>
   </si>
@@ -103,66 +103,6 @@
   </si>
   <si>
     <t>AM3</t>
-  </si>
-  <si>
-    <t>Male</t>
-  </si>
-  <si>
-    <t>Female</t>
-  </si>
-  <si>
-    <t>Ataxic</t>
-  </si>
-  <si>
-    <t>HD</t>
-  </si>
-  <si>
-    <t>PD</t>
-  </si>
-  <si>
-    <t>ALS</t>
-  </si>
-  <si>
-    <t>AF2</t>
-  </si>
-  <si>
-    <t>AF7</t>
-  </si>
-  <si>
-    <t>AF8</t>
-  </si>
-  <si>
-    <t>AM4</t>
-  </si>
-  <si>
-    <t>AM8</t>
-  </si>
-  <si>
-    <t>?</t>
-  </si>
-  <si>
-    <t>PDM15</t>
-  </si>
-  <si>
-    <t>PDM8</t>
-  </si>
-  <si>
-    <t>HDM12</t>
-  </si>
-  <si>
-    <t>ALSM7</t>
-  </si>
-  <si>
-    <t>ALSM8</t>
-  </si>
-  <si>
-    <t>ALSF6</t>
-  </si>
-  <si>
-    <t>ALSF2</t>
-  </si>
-  <si>
-    <t>Speaker Sex</t>
   </si>
 </sst>
 </file>
@@ -193,24 +133,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF889FF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF7DFFF8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -225,12 +153,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -555,7 +482,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9:I9"/>
+      <selection activeCell="E7" sqref="E6:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -570,12 +497,6 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H1" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -587,15 +508,6 @@
       <c r="C2">
         <v>6.66</v>
       </c>
-      <c r="F2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2">
-        <v>3</v>
-      </c>
-      <c r="H2">
-        <v>2</v>
-      </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
@@ -607,15 +519,6 @@
       <c r="C3">
         <v>3.1</v>
       </c>
-      <c r="F3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3">
-        <v>3</v>
-      </c>
-      <c r="H3">
-        <v>2</v>
-      </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
@@ -627,15 +530,6 @@
       <c r="C4">
         <v>5.78</v>
       </c>
-      <c r="F4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G4">
-        <v>3</v>
-      </c>
-      <c r="H4">
-        <v>2</v>
-      </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
@@ -647,15 +541,6 @@
       <c r="C5">
         <v>4.03</v>
       </c>
-      <c r="F5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5">
-        <v>2</v>
-      </c>
-      <c r="H5">
-        <v>3</v>
-      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
@@ -667,14 +552,6 @@
       <c r="C6">
         <v>9.74</v>
       </c>
-      <c r="G6">
-        <f>SUM(G2:G5)</f>
-        <v>11</v>
-      </c>
-      <c r="H6">
-        <f>SUM(H2:H5)</f>
-        <v>9</v>
-      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
@@ -708,18 +585,6 @@
       <c r="C9">
         <v>10.8</v>
       </c>
-      <c r="F9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G9" t="s">
-        <v>26</v>
-      </c>
-      <c r="H9" t="s">
-        <v>27</v>
-      </c>
-      <c r="I9" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
@@ -731,18 +596,6 @@
       <c r="C10">
         <v>3.86</v>
       </c>
-      <c r="F10" t="s">
-        <v>13</v>
-      </c>
-      <c r="G10" t="s">
-        <v>10</v>
-      </c>
-      <c r="H10" t="s">
-        <v>18</v>
-      </c>
-      <c r="I10" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
@@ -754,18 +607,6 @@
       <c r="C11">
         <v>6.29</v>
       </c>
-      <c r="F11" t="s">
-        <v>21</v>
-      </c>
-      <c r="G11" t="s">
-        <v>14</v>
-      </c>
-      <c r="H11" t="s">
-        <v>19</v>
-      </c>
-      <c r="I11" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
@@ -777,18 +618,6 @@
       <c r="C12">
         <v>5.75</v>
       </c>
-      <c r="F12" t="s">
-        <v>16</v>
-      </c>
-      <c r="G12" t="s">
-        <v>4</v>
-      </c>
-      <c r="H12" t="s">
-        <v>17</v>
-      </c>
-      <c r="I12" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
@@ -800,18 +629,6 @@
       <c r="C13" s="2">
         <v>10.199999999999999</v>
       </c>
-      <c r="F13" t="s">
-        <v>22</v>
-      </c>
-      <c r="G13" t="s">
-        <v>12</v>
-      </c>
-      <c r="H13" t="s">
-        <v>5</v>
-      </c>
-      <c r="I13" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
@@ -823,18 +640,6 @@
       <c r="C14">
         <v>2.82</v>
       </c>
-      <c r="F14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G14" t="s">
-        <v>11</v>
-      </c>
-      <c r="H14" t="s">
-        <v>20</v>
-      </c>
-      <c r="I14" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
@@ -846,21 +651,12 @@
       <c r="C15">
         <v>6.3</v>
       </c>
-      <c r="F15" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="I15" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="K15" t="s">
-        <v>42</v>
-      </c>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
@@ -872,21 +668,12 @@
       <c r="C16">
         <v>14.65</v>
       </c>
-      <c r="F16" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="I16" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="K16" s="4" t="s">
-        <v>23</v>
-      </c>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
@@ -898,21 +685,12 @@
       <c r="C17">
         <v>12.11</v>
       </c>
-      <c r="F17" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="I17" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="K17" s="3" t="s">
-        <v>24</v>
-      </c>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
@@ -924,18 +702,12 @@
       <c r="C18">
         <v>20.059999999999999</v>
       </c>
-      <c r="F18" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="H18" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
@@ -947,18 +719,12 @@
       <c r="C19" s="2">
         <v>5.49</v>
       </c>
-      <c r="F19" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>41</v>
-      </c>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">

</xml_diff>